<commit_message>
update common test case
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_CommonTest Case_v1.0_EN .xlsx
+++ b/WIP/Deliverable/Report3/VMN_CommonTest Case_v1.0_EN .xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="27320" windowHeight="15360" tabRatio="821"/>
+    <workbookView xWindow="260" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="821" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -454,15 +454,6 @@
   </si>
   <si>
     <t>Check 'Thoát'  when user login successfully</t>
-  </si>
-  <si>
-    <t>Check click on 'Dandelion'</t>
-  </si>
-  <si>
-    <t>Click on 'Dandelion'</t>
-  </si>
-  <si>
-    <t>1. Go to Homepage</t>
   </si>
   <si>
     <t>Security</t>
@@ -2302,7 +2293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2339,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="135" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D4" s="135"/>
       <c r="E4" s="135"/>
@@ -2347,7 +2338,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
@@ -2355,7 +2346,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="135" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D5" s="135"/>
       <c r="E5" s="135"/>
@@ -2363,7 +2354,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
@@ -2447,7 +2438,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -2803,7 +2794,7 @@
       </c>
       <c r="F3" s="142"/>
       <c r="G3" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H3" s="61"/>
     </row>
@@ -2821,7 +2812,7 @@
       </c>
       <c r="F4" s="142"/>
       <c r="G4" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H4" s="61"/>
     </row>
@@ -2924,7 +2915,7 @@
       </c>
       <c r="F11" s="72">
         <f>Common!C6</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" s="72">
         <f>Common!D6</f>
@@ -2932,7 +2923,7 @@
       </c>
       <c r="H11" s="73">
         <f>Common!E6</f>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2941,7 +2932,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="120" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D12" s="72">
         <f>Security!A6</f>
@@ -2970,7 +2961,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="120" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="72">
         <f>UI!A6</f>
@@ -3009,7 +3000,7 @@
       </c>
       <c r="F14" s="75">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="75">
         <f t="shared" si="0"/>
@@ -3017,7 +3008,7 @@
       </c>
       <c r="H14" s="75">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3102,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -3903,7 +3894,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="146"/>
       <c r="D4" s="146"/>
@@ -4424,24 +4415,24 @@
     </row>
     <row r="6" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6" s="114">
-        <f>COUNTIF(F11:G175,"Pass")</f>
+        <f>COUNTIF(F11:G174,"Pass")</f>
         <v>0</v>
       </c>
       <c r="B6" s="95">
-        <f>COUNTIF(F11:G622,"Fail")</f>
+        <f>COUNTIF(F11:G621,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C6" s="95">
         <f>E6-D6-B6-A6</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="96">
-        <f>COUNTIF(F11:G622,"N/A")</f>
+        <f>COUNTIF(F11:G621,"N/A")</f>
         <v>0</v>
       </c>
       <c r="E6" s="148">
-        <f>COUNTA(A11:A179)*2</f>
-        <v>12</v>
+        <f>COUNTA(A11:A178)*2</f>
+        <v>10</v>
       </c>
       <c r="F6" s="148"/>
       <c r="G6" s="148"/>
@@ -5745,13 +5736,13 @@
         <v>[User_login-2]</v>
       </c>
       <c r="B12" s="106" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C12" s="106" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D12" s="106" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E12" s="107"/>
       <c r="F12" s="106"/>
@@ -5769,10 +5760,10 @@
         <v>63</v>
       </c>
       <c r="C13" s="106" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D13" s="106" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E13" s="107"/>
       <c r="F13" s="106"/>
@@ -5787,13 +5778,13 @@
         <v>[User_login-4]</v>
       </c>
       <c r="B14" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="106" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="106" t="s">
+      <c r="D14" s="106" t="s">
         <v>124</v>
-      </c>
-      <c r="D14" s="106" t="s">
-        <v>127</v>
       </c>
       <c r="E14" s="107"/>
       <c r="F14" s="106"/>
@@ -5808,13 +5799,13 @@
         <v>[User_login-5]</v>
       </c>
       <c r="B15" s="106" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="106" t="s">
+      <c r="D15" s="106" t="s">
         <v>125</v>
-      </c>
-      <c r="D15" s="106" t="s">
-        <v>128</v>
       </c>
       <c r="E15" s="107"/>
       <c r="F15" s="106"/>
@@ -5829,13 +5820,13 @@
         <v>[User_login-6]</v>
       </c>
       <c r="B16" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="106" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="D16" s="106" t="s">
         <v>126</v>
-      </c>
-      <c r="D16" s="106" t="s">
-        <v>129</v>
       </c>
       <c r="E16" s="125"/>
       <c r="F16" s="106"/>
@@ -5844,25 +5835,7 @@
       <c r="I16" s="109"/>
       <c r="J16" s="98"/>
     </row>
-    <row r="17" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A17" s="125" t="str">
-        <f>IF(OR(B17&lt;&gt;"",D17&lt;E14&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[User_login-7]</v>
-      </c>
-      <c r="B17" s="106" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="106" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="106" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="125"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="109"/>
+    <row r="17" spans="10:10" ht="14.25" customHeight="1">
       <c r="J17" s="98"/>
     </row>
   </sheetData>
@@ -5879,10 +5852,10 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G18:G65247">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G17:G65246">
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F12:G17">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F12:G16">
       <formula1>$J$2:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -5904,8 +5877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -6185,7 +6158,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="145" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="145"/>
       <c r="D2" s="145"/>
@@ -6705,7 +6678,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="146"/>
       <c r="D4" s="146"/>
@@ -8530,7 +8503,7 @@
     <row r="11" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="128"/>
       <c r="B11" s="128" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" s="128"/>
       <c r="D11" s="128"/>
@@ -8546,13 +8519,13 @@
         <v>ID-2</v>
       </c>
       <c r="B12" s="106" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="106" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="106" t="s">
-        <v>135</v>
-      </c>
       <c r="D12" s="106" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="106"/>
@@ -8566,13 +8539,13 @@
         <v>ID-3</v>
       </c>
       <c r="B13" s="106" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C13" s="106" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D13" s="106" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E13" s="106"/>
       <c r="F13" s="106"/>
@@ -8586,13 +8559,13 @@
         <v>ID-4</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C14" s="106" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D14" s="106" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E14" s="106"/>
       <c r="F14" s="106"/>
@@ -8606,13 +8579,13 @@
         <v>ID-5</v>
       </c>
       <c r="B15" s="106" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C15" s="106" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D15" s="106" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" s="106"/>
       <c r="F15" s="106"/>
@@ -8623,7 +8596,7 @@
     <row r="16" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
       <c r="A16" s="128"/>
       <c r="B16" s="128" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C16" s="128"/>
       <c r="D16" s="128"/>
@@ -8639,13 +8612,13 @@
         <v>ID-6</v>
       </c>
       <c r="B17" s="106" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C17" s="106" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D17" s="106" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E17" s="106"/>
       <c r="F17" s="106"/>
@@ -8659,13 +8632,13 @@
         <v>ID-7</v>
       </c>
       <c r="B18" s="106" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C18" s="106" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D18" s="106" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E18" s="106"/>
       <c r="F18" s="106"/>
@@ -8680,13 +8653,13 @@
         <v>ID-8</v>
       </c>
       <c r="B19" s="106" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C19" s="106" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D19" s="106" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E19" s="106"/>
       <c r="F19" s="106"/>
@@ -8746,7 +8719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW24"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -9547,7 +9520,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="146"/>
       <c r="D4" s="146"/>
@@ -11371,7 +11344,7 @@
     <row r="11" spans="1:257" s="89" customFormat="1" ht="13">
       <c r="A11" s="128"/>
       <c r="B11" s="128" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" s="128"/>
       <c r="D11" s="128"/>
@@ -11387,13 +11360,13 @@
         <v>ID-2</v>
       </c>
       <c r="B12" s="106" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C12" s="106" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D12" s="106" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="106"/>
@@ -11407,13 +11380,13 @@
         <v>ID-3</v>
       </c>
       <c r="B13" s="106" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13" s="106" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D13" s="106" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E13" s="106"/>
       <c r="F13" s="106"/>
@@ -11427,13 +11400,13 @@
         <v>ID-4</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C14" s="106" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D14" s="106" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E14" s="106"/>
       <c r="F14" s="106"/>
@@ -11447,13 +11420,13 @@
         <v>ID-5</v>
       </c>
       <c r="B15" s="106" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" s="106" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D15" s="106" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E15" s="106"/>
       <c r="F15" s="106"/>
@@ -11467,13 +11440,13 @@
         <v>ID-6</v>
       </c>
       <c r="B16" s="106" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" s="106" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D16" s="106" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E16" s="106"/>
       <c r="F16" s="106"/>
@@ -11487,13 +11460,13 @@
         <v>ID-7</v>
       </c>
       <c r="B17" s="106" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C17" s="106" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D17" s="106" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E17" s="106"/>
       <c r="F17" s="106"/>
@@ -11507,13 +11480,13 @@
         <v>ID-8</v>
       </c>
       <c r="B18" s="106" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C18" s="106" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D18" s="106" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E18" s="106"/>
       <c r="F18" s="106"/>
@@ -11527,13 +11500,13 @@
         <v>ID-9</v>
       </c>
       <c r="B19" s="106" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C19" s="106" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D19" s="106" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E19" s="106"/>
       <c r="F19" s="106"/>
@@ -11547,13 +11520,13 @@
         <v>ID-10</v>
       </c>
       <c r="B20" s="106" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C20" s="106" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D20" s="106" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E20" s="106"/>
       <c r="F20" s="106"/>
@@ -11567,13 +11540,13 @@
         <v>ID-11</v>
       </c>
       <c r="B21" s="106" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" s="106" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D21" s="106" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E21" s="106"/>
       <c r="F21" s="106"/>
@@ -11587,13 +11560,13 @@
         <v>ID-12</v>
       </c>
       <c r="B22" s="106" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" s="106" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D22" s="106" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E22" s="106"/>
       <c r="F22" s="106"/>
@@ -11607,13 +11580,13 @@
         <v>ID-13</v>
       </c>
       <c r="B23" s="106" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23" s="106" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D23" s="106" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E23" s="106"/>
       <c r="F23" s="106"/>
@@ -11627,13 +11600,13 @@
         <v>ID-14</v>
       </c>
       <c r="B24" s="106" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" s="106" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D24" s="106" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E24" s="106"/>
       <c r="F24" s="106"/>

</xml_diff>